<commit_message>
Added protection to the sheets
</commit_message>
<xml_diff>
--- a/CSD_Daily_status.xlsx
+++ b/CSD_Daily_status.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bench_status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C6630-9437-4B27-9E95-FDCE22FB68F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74242D8-3E07-457B-9C1A-09C2F430E99C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kWFHmNGnqNKFGijJvfabpUvI1EKsE0VWrBedqe5ViS0byVu+xezzeGL/1vzrR4TYE2jxLdUqJ5l+ZYPmwCdWxg==" workbookSaltValue="C6ZiAuHqpsuNFxKAC/BOLA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="status-18-03-2020" sheetId="14" r:id="rId1"/>
@@ -30,6 +31,7 @@
     <sheet name="Status-07-04-2020" sheetId="31" r:id="rId15"/>
     <sheet name="Status-10-04-2020" sheetId="32" r:id="rId16"/>
     <sheet name="Status-17-04-2020" sheetId="34" r:id="rId17"/>
+    <sheet name="Status-20-04-2020" sheetId="35" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="222">
   <si>
     <t>Date</t>
   </si>
@@ -20499,7 +20501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -20887,7 +20889,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -21042,6 +21044,508 @@
       <c r="D30" s="5" t="s">
         <v>215</v>
       </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="35">
+        <v>30</v>
+      </c>
+      <c r="B31" s="33">
+        <v>154223</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="pCQypCgrCIGaj0R5jruDogmD1nva92vodDdkBb/0qqPN0/uJpfkjdU9RzLF0RGBfP8/w1jW70Gd8Ji6BpvBRdA==" saltValue="4yBEc5XeWsNGVHPemtIR9g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB8ECD0-792E-4F36-AA74-889257A30E5D}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.6328125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="55">
+        <v>94597</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="14">
+        <v>9</v>
+      </c>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>67908</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>156137</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="55">
+        <v>189815</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="55">
+        <v>119065</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="16">
+        <v>9</v>
+      </c>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>185010</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>154447</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="18">
+        <v>9</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18">
+        <v>9</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="58">
+        <v>175816</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="51">
+        <v>9</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11" s="55">
+        <v>191221</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="18">
+        <v>9</v>
+      </c>
+      <c r="F11" s="50"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="14">
+        <v>11</v>
+      </c>
+      <c r="B12" s="55">
+        <v>46014906</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="18">
+        <v>9</v>
+      </c>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="27">
+        <v>156635</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="18">
+        <v>9</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="27">
+        <v>168293</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="18">
+        <v>9</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="14">
+        <v>14</v>
+      </c>
+      <c r="B15" s="27">
+        <v>151146</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="27">
+        <v>156996</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E16" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="27">
+        <v>185599</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="14">
+        <v>17</v>
+      </c>
+      <c r="B18" s="27">
+        <v>96340</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="14">
+        <v>18</v>
+      </c>
+      <c r="B19" s="27">
+        <v>108444</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12">
+        <v>139666</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="51">
+        <v>9</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="27">
+        <v>141023</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="14">
+        <v>21</v>
+      </c>
+      <c r="B22" s="27">
+        <v>178684</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="14">
+        <v>22</v>
+      </c>
+      <c r="B23" s="27">
+        <v>187084</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="14">
+        <v>23</v>
+      </c>
+      <c r="B24" s="27">
+        <v>46013133</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="E24" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="14">
+        <v>24</v>
+      </c>
+      <c r="B25" s="27">
+        <v>151158</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="14">
+        <v>25</v>
+      </c>
+      <c r="B26" s="27">
+        <v>142742</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="11">
+        <v>26</v>
+      </c>
+      <c r="B27" s="12">
+        <v>142584</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
+        <v>27</v>
+      </c>
+      <c r="B28" s="12">
+        <v>100578</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="11">
+        <v>28</v>
+      </c>
+      <c r="B29" s="12">
+        <v>176569</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="11">
+        <v>29</v>
+      </c>
+      <c r="B30" s="12">
+        <v>190871</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="35">

</xml_diff>